<commit_message>
Se incluye un reporte con 17 preguntas.
</commit_message>
<xml_diff>
--- a/Moldes/Reporte.xlsx
+++ b/Moldes/Reporte.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte" sheetId="1" state="visible" r:id="rId2"/>
@@ -79,7 +79,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -122,6 +122,21 @@
       <b val="true"/>
       <sz val="16"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -304,11 +319,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -411,16 +426,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.73828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="3" style="0" width="12.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="3" style="0" width="12.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -446,7 +461,7 @@
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="str">
-        <f aca="false">IFERROR(INDEX(Respuestas!A1:Z400,MATCH(C1,Respuestas!A1:A400,0)+1,16),"")</f>
+        <f aca="false">IFERROR(INDEX(Respuestas!A1:Z400,MATCH(C1,Respuestas!A1:A400,0)+1,19),"")</f>
         <v/>
       </c>
       <c r="D2" s="6"/>
@@ -462,7 +477,7 @@
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="9" t="str">
-        <f aca="false">IFERROR(INDEX(Respuestas!A1:Z400,MATCH(C1,Respuestas!A1:A400,0)+1,17),"persona no encontrada")</f>
+        <f aca="false">IFERROR(INDEX(Respuestas!A1:Z400,MATCH(C1,Respuestas!A1:A400,0)+1,20),"persona no encontrada")</f>
         <v>persona no encontrada</v>
       </c>
       <c r="D3" s="9"/>
@@ -514,6 +529,15 @@
       <c r="P4" s="12" t="n">
         <v>14</v>
       </c>
+      <c r="Q4" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="R4" s="12" t="n">
+        <v>16</v>
+      </c>
+      <c r="S4" s="12" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
@@ -576,6 +600,18 @@
         <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0),15),"")</f>
         <v/>
       </c>
+      <c r="Q5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0),16),"")</f>
+        <v/>
+      </c>
+      <c r="R5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0),17),"")</f>
+        <v/>
+      </c>
+      <c r="S5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0),18),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
@@ -638,6 +674,18 @@
         <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+2,15),"")</f>
         <v/>
       </c>
+      <c r="Q6" s="14" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+2,16),"")</f>
+        <v/>
+      </c>
+      <c r="R6" s="14" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+2,17),"")</f>
+        <v/>
+      </c>
+      <c r="S6" s="14" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+2,18),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="15" t="s">
@@ -698,6 +746,18 @@
       </c>
       <c r="P7" s="16" t="str">
         <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+1,15),"")</f>
+        <v/>
+      </c>
+      <c r="Q7" s="16" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+1,16),"")</f>
+        <v/>
+      </c>
+      <c r="R7" s="16" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+1,17),"")</f>
+        <v/>
+      </c>
+      <c r="S7" s="16" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+1,18),"")</f>
         <v/>
       </c>
     </row>
@@ -765,131 +825,116 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="Q2:Q187"/>
+  <dimension ref="T2:T162"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="1" style="18" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="1" style="18" width="10.72"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="53" style="18" width="8.67"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q2" s="19"/>
+      <c r="T2" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q7" s="19"/>
+      <c r="T7" s="19"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q12" s="19"/>
+      <c r="T12" s="19"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q17" s="19"/>
+      <c r="T17" s="19"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q22" s="19"/>
+      <c r="T22" s="19"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q27" s="19"/>
+      <c r="T27" s="19"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q32" s="19"/>
+      <c r="T32" s="19"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q37" s="19"/>
+      <c r="T37" s="19"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q42" s="19"/>
+      <c r="T42" s="19"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q47" s="19"/>
+      <c r="T47" s="19"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q52" s="19"/>
+      <c r="T52" s="19"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q57" s="19"/>
+      <c r="T57" s="19"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q62" s="19"/>
+      <c r="T62" s="19"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q67" s="19"/>
+      <c r="T67" s="19"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q72" s="19"/>
+      <c r="T72" s="19"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q77" s="19"/>
+      <c r="T77" s="19"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q82" s="19"/>
+      <c r="T82" s="19"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q87" s="19"/>
+      <c r="T87" s="19"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q92" s="19"/>
+      <c r="T92" s="19"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q97" s="19"/>
+      <c r="T97" s="19"/>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q102" s="19"/>
+      <c r="T102" s="19"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q107" s="19"/>
+      <c r="T107" s="19"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q112" s="19"/>
+      <c r="T112" s="19"/>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q117" s="19"/>
+      <c r="T117" s="19"/>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q122" s="19"/>
+      <c r="T122" s="19"/>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q127" s="19"/>
+      <c r="T127" s="19"/>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q132" s="19"/>
+      <c r="T132" s="19"/>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q137" s="19"/>
+      <c r="T137" s="19"/>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q142" s="19"/>
+      <c r="T142" s="19"/>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q147" s="19"/>
+      <c r="T147" s="19"/>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q152" s="19"/>
+      <c r="T152" s="19"/>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q157" s="19"/>
+      <c r="T157" s="19"/>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q162" s="19"/>
-    </row>
-    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q167" s="19"/>
-    </row>
-    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q172" s="19"/>
-    </row>
-    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q177" s="19"/>
-    </row>
-    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q182" s="19"/>
-    </row>
-    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q187" s="19"/>
+      <c r="T162" s="19"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Se agregan un mont\'on de preguntas al reporte.
</commit_message>
<xml_diff>
--- a/Moldes/Reporte.xlsx
+++ b/Moldes/Reporte.xlsx
@@ -79,7 +79,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -122,21 +122,6 @@
       <b val="true"/>
       <sz val="16"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -246,7 +231,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -315,15 +300,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -426,13 +415,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:AM10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.73828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="3" style="0" width="12.21"/>
@@ -461,7 +450,7 @@
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="str">
-        <f aca="false">IFERROR(INDEX(Respuestas!A1:Z400,MATCH(C1,Respuestas!A1:A400,0)+1,19),"")</f>
+        <f aca="false">IFERROR(INDEX(Respuestas!A1:DZ400,MATCH(C1,Respuestas!A1:A400,0)+1,39),"")</f>
         <v/>
       </c>
       <c r="D2" s="6"/>
@@ -477,7 +466,7 @@
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="9" t="str">
-        <f aca="false">IFERROR(INDEX(Respuestas!A1:Z400,MATCH(C1,Respuestas!A1:A400,0)+1,20),"persona no encontrada")</f>
+        <f aca="false">IFERROR(INDEX(Respuestas!A1:DZ400,MATCH(C1,Respuestas!A1:A400,0)+1,40),"persona no encontrada")</f>
         <v>persona no encontrada</v>
       </c>
       <c r="D3" s="9"/>
@@ -538,6 +527,66 @@
       <c r="S4" s="12" t="n">
         <v>17</v>
       </c>
+      <c r="T4" s="12" t="n">
+        <v>18</v>
+      </c>
+      <c r="U4" s="12" t="n">
+        <v>19</v>
+      </c>
+      <c r="V4" s="12" t="n">
+        <v>20</v>
+      </c>
+      <c r="W4" s="12" t="n">
+        <v>21</v>
+      </c>
+      <c r="X4" s="12" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y4" s="12" t="n">
+        <v>23</v>
+      </c>
+      <c r="Z4" s="12" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA4" s="12" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB4" s="12" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC4" s="12" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD4" s="12" t="n">
+        <v>28</v>
+      </c>
+      <c r="AE4" s="12" t="n">
+        <v>29</v>
+      </c>
+      <c r="AF4" s="12" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG4" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH4" s="12" t="n">
+        <v>32</v>
+      </c>
+      <c r="AI4" s="12" t="n">
+        <v>33</v>
+      </c>
+      <c r="AJ4" s="12" t="n">
+        <v>34</v>
+      </c>
+      <c r="AK4" s="12" t="n">
+        <v>35</v>
+      </c>
+      <c r="AL4" s="12" t="n">
+        <v>36</v>
+      </c>
+      <c r="AM4" s="12" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
@@ -612,6 +661,86 @@
         <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0),18),"")</f>
         <v/>
       </c>
+      <c r="T5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0),19),"")</f>
+        <v/>
+      </c>
+      <c r="U5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0),20),"")</f>
+        <v/>
+      </c>
+      <c r="V5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0),21),"")</f>
+        <v/>
+      </c>
+      <c r="W5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0),22),"")</f>
+        <v/>
+      </c>
+      <c r="X5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0),23),"")</f>
+        <v/>
+      </c>
+      <c r="Y5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0),24),"")</f>
+        <v/>
+      </c>
+      <c r="Z5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$Z$400,MATCH($C$1,Respuestas!$A$1:$A$400,0),25),"")</f>
+        <v/>
+      </c>
+      <c r="AA5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$Z$400,MATCH($C$1,Respuestas!$A$1:$A$400,0),26),"")</f>
+        <v/>
+      </c>
+      <c r="AB5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0),27),"")</f>
+        <v/>
+      </c>
+      <c r="AC5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0),28),"")</f>
+        <v/>
+      </c>
+      <c r="AD5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0),29),"")</f>
+        <v/>
+      </c>
+      <c r="AE5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0),30),"")</f>
+        <v/>
+      </c>
+      <c r="AF5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0),31),"")</f>
+        <v/>
+      </c>
+      <c r="AG5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0),32),"")</f>
+        <v/>
+      </c>
+      <c r="AH5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0),33),"")</f>
+        <v/>
+      </c>
+      <c r="AI5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0),34),"")</f>
+        <v/>
+      </c>
+      <c r="AJ5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0),35),"")</f>
+        <v/>
+      </c>
+      <c r="AK5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0),36),"")</f>
+        <v/>
+      </c>
+      <c r="AL5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0),37),"")</f>
+        <v/>
+      </c>
+      <c r="AM5" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0),38),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
@@ -686,6 +815,86 @@
         <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+2,18),"")</f>
         <v/>
       </c>
+      <c r="T6" s="14" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+2,19),"")</f>
+        <v/>
+      </c>
+      <c r="U6" s="14" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+2,20),"")</f>
+        <v/>
+      </c>
+      <c r="V6" s="14" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+2,21),"")</f>
+        <v/>
+      </c>
+      <c r="W6" s="14" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+2,22),"")</f>
+        <v/>
+      </c>
+      <c r="X6" s="14" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+2,23),"")</f>
+        <v/>
+      </c>
+      <c r="Y6" s="14" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+2,24),"")</f>
+        <v/>
+      </c>
+      <c r="Z6" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$Z$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+2,25),"")</f>
+        <v/>
+      </c>
+      <c r="AA6" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$Z$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+2,26),"")</f>
+        <v/>
+      </c>
+      <c r="AB6" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+2,27),"")</f>
+        <v/>
+      </c>
+      <c r="AC6" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+2,28),"")</f>
+        <v/>
+      </c>
+      <c r="AD6" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+2,29),"")</f>
+        <v/>
+      </c>
+      <c r="AE6" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+2,30),"")</f>
+        <v/>
+      </c>
+      <c r="AF6" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+2,31),"")</f>
+        <v/>
+      </c>
+      <c r="AG6" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+2,32),"")</f>
+        <v/>
+      </c>
+      <c r="AH6" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+2,33),"")</f>
+        <v/>
+      </c>
+      <c r="AI6" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+2,34),"")</f>
+        <v/>
+      </c>
+      <c r="AJ6" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+2,35),"")</f>
+        <v/>
+      </c>
+      <c r="AK6" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+2,36),"")</f>
+        <v/>
+      </c>
+      <c r="AL6" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+2,37),"")</f>
+        <v/>
+      </c>
+      <c r="AM6" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+2,38),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="15" t="s">
@@ -760,33 +969,113 @@
         <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+1,18),"")</f>
         <v/>
       </c>
+      <c r="T7" s="17" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+1,19),"")</f>
+        <v/>
+      </c>
+      <c r="U7" s="17" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+1,20),"")</f>
+        <v/>
+      </c>
+      <c r="V7" s="17" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+1,21),"")</f>
+        <v/>
+      </c>
+      <c r="W7" s="17" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+1,22),"")</f>
+        <v/>
+      </c>
+      <c r="X7" s="17" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+1,23),"")</f>
+        <v/>
+      </c>
+      <c r="Y7" s="17" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+1,24),"")</f>
+        <v/>
+      </c>
+      <c r="Z7" s="17" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+1,25),"")</f>
+        <v/>
+      </c>
+      <c r="AA7" s="17" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!A$1:Z$400,MATCH(C$1,Respuestas!A$1:A$400,0)+1,26),"")</f>
+        <v/>
+      </c>
+      <c r="AB7" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+1,27),"")</f>
+        <v/>
+      </c>
+      <c r="AC7" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+1,28),"")</f>
+        <v/>
+      </c>
+      <c r="AD7" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+1,29),"")</f>
+        <v/>
+      </c>
+      <c r="AE7" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+1,30),"")</f>
+        <v/>
+      </c>
+      <c r="AF7" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+1,31),"")</f>
+        <v/>
+      </c>
+      <c r="AG7" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+1,32),"")</f>
+        <v/>
+      </c>
+      <c r="AH7" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+1,33),"")</f>
+        <v/>
+      </c>
+      <c r="AI7" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+1,34),"")</f>
+        <v/>
+      </c>
+      <c r="AJ7" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+1,35),"")</f>
+        <v/>
+      </c>
+      <c r="AK7" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+1,36),"")</f>
+        <v/>
+      </c>
+      <c r="AL7" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+1,37),"")</f>
+        <v/>
+      </c>
+      <c r="AM7" s="12" t="str">
+        <f aca="false">IFERROR(INDEX(Respuestas!$A$1:$DZ$400,MATCH($C$1,Respuestas!$A$1:$A$400,0)+1,38),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -812,7 +1101,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -825,121 +1114,79 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="T2:T162"/>
+  <dimension ref="AN2:AN92"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="1" style="18" width="10.72"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="53" style="18" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="1" style="19" width="10.72"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="53" style="19" width="8.61"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T2" s="19"/>
+      <c r="AN2" s="20"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T7" s="19"/>
+      <c r="AN7" s="20"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T12" s="19"/>
+      <c r="AN12" s="20"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T17" s="19"/>
+      <c r="AN17" s="20"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T22" s="19"/>
+      <c r="AN22" s="20"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T27" s="19"/>
+      <c r="AN27" s="20"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T32" s="19"/>
+      <c r="AN32" s="20"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T37" s="19"/>
+      <c r="AN37" s="20"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T42" s="19"/>
+      <c r="AN42" s="20"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T47" s="19"/>
+      <c r="AN47" s="20"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T52" s="19"/>
+      <c r="AN52" s="20"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T57" s="19"/>
+      <c r="AN57" s="20"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T62" s="19"/>
+      <c r="AN62" s="20"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T67" s="19"/>
+      <c r="AN67" s="20"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T72" s="19"/>
+      <c r="AN72" s="20"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T77" s="19"/>
+      <c r="AN77" s="20"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T82" s="19"/>
+      <c r="AN82" s="20"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T87" s="19"/>
+      <c r="AN87" s="20"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T92" s="19"/>
-    </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T97" s="19"/>
-    </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T102" s="19"/>
-    </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T107" s="19"/>
-    </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T112" s="19"/>
-    </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T117" s="19"/>
-    </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T122" s="19"/>
-    </row>
-    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T127" s="19"/>
-    </row>
-    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T132" s="19"/>
-    </row>
-    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T137" s="19"/>
-    </row>
-    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T142" s="19"/>
-    </row>
-    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T147" s="19"/>
-    </row>
-    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T152" s="19"/>
-    </row>
-    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T157" s="19"/>
-    </row>
-    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T162" s="19"/>
+      <c r="AN92" s="20"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>